<commit_message>
updated Annullamento and testPlan
</commit_message>
<xml_diff>
--- a/docs/tp/Clients/Clients - Censimenti.xlsx
+++ b/docs/tp/Clients/Clients - Censimenti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TA\matrix-web-fe-tests\docs\tp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5257E64C-18DB-499C-90EC-E89281291B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A66734-C560-4C17-9BFC-495F7A686404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15900" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
+    <workbookView xWindow="-19320" yWindow="660" windowWidth="19440" windowHeight="15000" xr2:uid="{BE46A6EB-3E52-4087-BE1D-BF4A8643FA88}"/>
   </bookViews>
   <sheets>
     <sheet name="Bobo" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
   <si>
     <t>Oboe Andrea (Leased Employee)</t>
   </si>
@@ -210,13 +210,19 @@
   </si>
   <si>
     <t xml:space="preserve">Verificre che l'unico venga stampato correttamente </t>
+  </si>
+  <si>
+    <t>Area Path</t>
+  </si>
+  <si>
+    <t>Allianz Projects\Digital Interaction\Allianz Matrix Web\Clients</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +254,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,8 +285,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -298,13 +315,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,6 +346,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -635,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1AEFEBA-728D-4FDD-9B3D-F6BE0E3793BC}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I17"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,9 +684,10 @@
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -682,8 +715,11 @@
       <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -711,8 +747,11 @@
       <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -740,8 +779,11 @@
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -769,8 +811,11 @@
       <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -798,8 +843,11 @@
       <c r="I5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -827,8 +875,11 @@
       <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -856,8 +907,11 @@
       <c r="I7" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="J7" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -885,8 +939,11 @@
       <c r="I8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="J8" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -914,8 +971,11 @@
       <c r="I9" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
@@ -943,8 +1003,11 @@
       <c r="I10" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J10" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -972,8 +1035,11 @@
       <c r="I11" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J11" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>46</v>
       </c>
@@ -1001,8 +1067,11 @@
       <c r="I12" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="52.5" x14ac:dyDescent="0.25">
+      <c r="J12" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1030,8 +1099,11 @@
       <c r="I13" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
@@ -1059,8 +1131,11 @@
       <c r="I14" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="J14" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>49</v>
       </c>
@@ -1088,8 +1163,11 @@
       <c r="I15" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="J15" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>50</v>
       </c>
@@ -1117,8 +1195,11 @@
       <c r="I16" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J16" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>53</v>
       </c>
@@ -1145,6 +1226,9 @@
       </c>
       <c r="I17" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>